<commit_message>
LITE-25724: Fix line item report for fulfillment
</commit_message>
<xml_diff>
--- a/reports/fulfillment_requests_line_item/templates/xlsx/template.xlsx
+++ b/reports/fulfillment_requests_line_item/templates/xlsx/template.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11220"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11120"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-cli/cnctcli/reports/connect-reports/reports/fulfillment_requests/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marc1/Documents/Connect/connect-reports/reports/fulfillment_requests_line_item/templates/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5647451-DA08-964B-975C-B87F08E07227}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96594978-8A1A-2341-9849-BF41453BB323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36260" yWindow="500" windowWidth="35840" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="35840" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AG$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AH$1</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Request ID</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>Updated At</t>
+  </si>
+  <si>
+    <t>Asset Status</t>
   </si>
 </sst>
 </file>
@@ -468,48 +471,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AG1"/>
+  <dimension ref="A1:AH1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="4" width="21.1640625" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="21.1640625" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="9" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="10" customWidth="1"/>
-    <col min="13" max="13" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="20" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="17" max="17" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="18" max="18" width="20" customWidth="1"/>
-    <col min="19" max="19" width="19.33203125" customWidth="1" outlineLevel="1"/>
-    <col min="20" max="20" width="45.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="21" max="21" width="20" customWidth="1"/>
-    <col min="22" max="22" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="45.83203125" customWidth="1"/>
-    <col min="24" max="24" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="25" max="25" width="45.83203125" customWidth="1"/>
-    <col min="26" max="26" width="20" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="45.83203125" customWidth="1"/>
-    <col min="28" max="28" width="25.83203125" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="20" customWidth="1"/>
-    <col min="30" max="30" width="14" customWidth="1"/>
-    <col min="31" max="31" width="15" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="45.83203125" customWidth="1"/>
-    <col min="33" max="33" width="18.5" customWidth="1"/>
+    <col min="2" max="3" width="15" customWidth="1"/>
+    <col min="4" max="5" width="21.1640625" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="10" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="20" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="18" max="18" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="19" max="19" width="20" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" customWidth="1" outlineLevel="1"/>
+    <col min="21" max="21" width="45.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="20" customWidth="1"/>
+    <col min="23" max="23" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="24" max="24" width="45.83203125" customWidth="1"/>
+    <col min="25" max="25" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="45.83203125" customWidth="1"/>
+    <col min="27" max="27" width="20" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="45.83203125" customWidth="1"/>
+    <col min="29" max="29" width="25.83203125" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="20" customWidth="1"/>
+    <col min="31" max="31" width="14" customWidth="1"/>
+    <col min="32" max="32" width="15" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="45.83203125" customWidth="1"/>
+    <col min="34" max="34" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -517,101 +520,104 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AG1" s="1" t="s">
-        <v>20</v>
+      <c r="AH1" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AG1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
+  <autoFilter ref="A1:AH1" xr:uid="{444A851A-3A6C-984B-A410-97137E4DF2E6}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>